<commit_message>
adding example of why you might want NA values
</commit_message>
<xml_diff>
--- a/data/cleaning_diet_data.xlsx
+++ b/data/cleaning_diet_data.xlsx
@@ -405,7 +405,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>Ginger</t>
         </is>
       </c>
       <c r="C3">
@@ -459,7 +459,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Peppermint</t>
+          <t>peppermint</t>
         </is>
       </c>
       <c r="C6">
@@ -477,7 +477,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>ginger</t>
         </is>
       </c>
       <c r="C7">

</xml_diff>